<commit_message>
revert stupid code to even stupider code
</commit_message>
<xml_diff>
--- a/combined_model.xlsx
+++ b/combined_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/Library/CloudStorage/iCloud Drive/Documents/Summer/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EF5E92-20DE-F846-BA77-CE97818048FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1554B539-3395-5246-ABCB-0FD7BC0DBA3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3138,8 +3138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:UR124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -6901,7 +6901,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="49">
         <v>1</v>
@@ -23319,7 +23319,7 @@
         <v>28</v>
       </c>
       <c r="D40" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="49">
         <v>1</v>
@@ -26817,7 +26817,7 @@
       </c>
       <c r="C46" s="49"/>
       <c r="D46" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="49">
         <v>1</v>
@@ -37339,7 +37339,7 @@
         <v>97</v>
       </c>
       <c r="D65" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" s="49">
         <v>1</v>
@@ -43759,7 +43759,7 @@
         <v>43</v>
       </c>
       <c r="D76" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E76" s="49">
         <v>1</v>
@@ -44489,7 +44489,7 @@
         <v>86</v>
       </c>
       <c r="D82" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82" s="49">
         <v>1</v>
@@ -44639,7 +44639,7 @@
         <v>79</v>
       </c>
       <c r="D87" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87" s="49">
         <v>1</v>
@@ -45401,7 +45401,7 @@
         <v>64</v>
       </c>
       <c r="D113" s="49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113" s="49">
         <v>1</v>
@@ -45761,7 +45761,7 @@
   <dimension ref="A1:AZ181"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>